<commit_message>
Many hard things added
</commit_message>
<xml_diff>
--- a/EasyWay.Core/Data/Data.xlsx
+++ b/EasyWay.Core/Data/Data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSbook\RiderProjects\EasyWay.UI\EasyWay.Core\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E9A6F2-1206-4572-B20A-0FED260D5F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CE275F-4EE0-4AF4-802B-D7A4C5CF96C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3732" yWindow="-17388" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -40,6 +41,12 @@
   </si>
   <si>
     <t>Bob</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -357,37 +364,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F903A5-2F9D-4016-B3AB-3F569BA2A8B4}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Submodel own state understanding.
</commit_message>
<xml_diff>
--- a/EasyWay.Core/Data/Data.xlsx
+++ b/EasyWay.Core/Data/Data.xlsx
@@ -331,33 +331,57 @@
     </row>
     <row>
       <c r="A2" t="str">
+        <v>743</v>
+      </c>
+      <c r="B2" t="str">
+        <v>sjvcskjk</v>
+      </c>
+    </row>
+    <row>
+      <c r="A3" t="str">
+        <v>452</v>
+      </c>
+      <c r="B3" t="str">
+        <v>hfc</v>
+      </c>
+    </row>
+    <row>
+      <c r="A4" t="str">
+        <v>9</v>
+      </c>
+      <c r="B4" t="str">
+        <v>cffcgg</v>
+      </c>
+    </row>
+    <row>
+      <c r="A5" t="str">
+        <v>867</v>
+      </c>
+      <c r="B5" t="str">
+        <v>dgxdd</v>
+      </c>
+    </row>
+    <row>
+      <c r="A6" t="str">
         <v>801</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B6" t="str">
         <v>sa</v>
       </c>
     </row>
     <row>
-      <c r="A3" t="str">
+      <c r="A7" t="str">
         <v>245</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B7" t="str">
         <v>sad</v>
       </c>
     </row>
     <row>
-      <c r="A4" t="str">
-        <v>410</v>
-      </c>
-      <c r="B4" t="str">
-        <v>asd</v>
-      </c>
-    </row>
-    <row>
-      <c r="A5" t="str">
+      <c r="A8" t="str">
         <v>788</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B8" t="str">
         <v>sadsa</v>
       </c>
     </row>

</xml_diff>